<commit_message>
update spreadsheet for PD 47
</commit_message>
<xml_diff>
--- a/Standards_Program/TC_policy_directives/policy_directives.xlsx
+++ b/Standards_Program/TC_policy_directives/policy_directives.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/policy/Standards_Program/TC_policy_directives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/policy/Standards_Program/TC_policy_directives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10941B3B-7215-1D42-BE96-2182E43619B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B88A6F4-3A78-2B4B-A123-673D82DA8B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27720" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
   <si>
     <t>date</t>
   </si>
@@ -761,6 +761,18 @@
   </si>
   <si>
     <t>standard, coordinate reference system</t>
+  </si>
+  <si>
+    <t>standard, collaboration</t>
+  </si>
+  <si>
+    <t>All OGC API SWGs will work on their respective standards with other OGC API SWGs and the OWS Common SWG and report on the interaction with those SWGs to ensure coherence (with respect to OGC Web API Guidelines, OGC API - Common, and reusability of extensions) of standards in advance of OAB review. OAB will develop a template for the review. If the OAB determines that sufficient review has not taken place, the submitting SWG will be instructed to perform further review.
+OAB will deliver a template by the end of 2019. OGC API SWGs currently working will perform coherence review as described above over at least the time required to receive the template.
+This motion does not preclude formation of a SWG, it only applies to work undertaken by an existing SWG.
+This coordination effort occurs after the formation of a SWG and before OAB review of a candidate standard for public RFC.</t>
+  </si>
+  <si>
+    <t>OGC API coordination</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2151,6 +2163,26 @@
         <v>165</v>
       </c>
     </row>
+    <row r="48" spans="1:7" ht="221">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>43770</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add PD 50, update PD 47 and spreadsheet
</commit_message>
<xml_diff>
--- a/Standards_Program/TC_policy_directives/policy_directives.xlsx
+++ b/Standards_Program/TC_policy_directives/policy_directives.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/policy/Standards_Program/TC_policy_directives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DF1EF8-7E45-4D41-98CF-9517B39730EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B2B977-B1B1-284D-AC24-4C29481A34C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27720" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="176">
   <si>
     <t>date</t>
   </si>
@@ -788,6 +788,9 @@
   </si>
   <si>
     <t>see adoc file</t>
+  </si>
+  <si>
+    <t>standard, template, collaboration</t>
   </si>
 </sst>
 </file>
@@ -847,7 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -865,6 +868,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1148,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2250,6 +2256,26 @@
         <v>174</v>
       </c>
     </row>
+    <row r="51" spans="1:7" ht="34">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7">
+        <v>44281</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>